<commit_message>
New plotting functions, Matlab for Halfwidth data from Dr. Creuziger
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AveragedIntensities-SRP/Alpha1F-HW20.xlsx
+++ b/JupyterNotebooks/AveragedIntensities-SRP/Alpha1F-HW20.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>HKL</t>
   </si>
@@ -31,6 +31,18 @@
     <t>Spiral</t>
   </si>
   <si>
+    <t>OffsetF</t>
+  </si>
+  <si>
+    <t>OffsetA</t>
+  </si>
+  <si>
+    <t>RD Single</t>
+  </si>
+  <si>
+    <t>TD Single</t>
+  </si>
+  <si>
     <t>HexGrid-90degTilt5degRes</t>
   </si>
   <si>
@@ -59,6 +71,9 @@
   </si>
   <si>
     <t>1Pair-A</t>
+  </si>
+  <si>
+    <t>1Pair-B</t>
   </si>
   <si>
     <t>2Pairs-A</t>
@@ -440,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -501,8 +516,11 @@
       <c r="S1" s="1">
         <v>17</v>
       </c>
+      <c r="T1" s="1">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -510,58 +528,61 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="R2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="S2" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="T2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -569,58 +590,61 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.9123414985590778</v>
+        <v>0.9153170028818444</v>
       </c>
       <c r="D3">
-        <v>1.255079250720461</v>
+        <v>1.251433717579251</v>
       </c>
       <c r="E3">
-        <v>0.9432204610951008</v>
+        <v>0.9428458213256484</v>
       </c>
       <c r="F3">
-        <v>0.9123414985590778</v>
+        <v>0.9153170028818444</v>
       </c>
       <c r="G3">
-        <v>1.133011527377522</v>
+        <v>1.132118155619597</v>
       </c>
       <c r="H3">
-        <v>0.8603602305475504</v>
+        <v>0.8583933717579251</v>
       </c>
       <c r="I3">
-        <v>0.935835734870317</v>
+        <v>0.9364337175792508</v>
       </c>
       <c r="J3">
-        <v>1.255079250720461</v>
+        <v>1.251433717579251</v>
       </c>
       <c r="K3">
-        <v>0.9123414985590778</v>
+        <v>0.9153170028818444</v>
       </c>
       <c r="L3">
-        <v>1.099149855907781</v>
+        <v>0.9428458213256484</v>
       </c>
       <c r="M3">
-        <v>1.099149855907781</v>
+        <v>1.09713976945245</v>
       </c>
       <c r="N3">
-        <v>1.110437079731028</v>
+        <v>1.09713976945245</v>
       </c>
       <c r="O3">
-        <v>1.036880403458213</v>
+        <v>1.108799231508165</v>
       </c>
       <c r="P3">
-        <v>1.036880403458213</v>
+        <v>1.036532180595581</v>
       </c>
       <c r="Q3">
-        <v>1.005745677233429</v>
+        <v>1.036532180595581</v>
       </c>
       <c r="R3">
-        <v>1.005745677233429</v>
+        <v>1.006228386167147</v>
       </c>
       <c r="S3">
-        <v>1.006641450528338</v>
+        <v>1.006228386167147</v>
+      </c>
+      <c r="T3">
+        <v>1.006090297790586</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -628,58 +652,61 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.9947256494691598</v>
+        <v>0.9967415414473634</v>
       </c>
       <c r="D4">
-        <v>1.017176742625276</v>
+        <v>1.014824979741739</v>
       </c>
       <c r="E4">
-        <v>0.990052623194252</v>
+        <v>0.989674153860961</v>
       </c>
       <c r="F4">
-        <v>0.9947256494691598</v>
+        <v>0.9967415414473634</v>
       </c>
       <c r="G4">
-        <v>1.010820521087429</v>
+        <v>1.010550431152634</v>
       </c>
       <c r="H4">
-        <v>0.9774811073295212</v>
+        <v>0.9755317116315174</v>
       </c>
       <c r="I4">
-        <v>0.9904684197333647</v>
+        <v>0.9907461123635702</v>
       </c>
       <c r="J4">
-        <v>1.017176742625276</v>
+        <v>1.014824979741739</v>
       </c>
       <c r="K4">
-        <v>0.9947256494691598</v>
+        <v>0.9967415414473634</v>
       </c>
       <c r="L4">
-        <v>1.003614682909764</v>
+        <v>0.989674153860961</v>
       </c>
       <c r="M4">
-        <v>1.003614682909764</v>
+        <v>1.00224956680135</v>
       </c>
       <c r="N4">
-        <v>1.006016628968986</v>
+        <v>1.00224956680135</v>
       </c>
       <c r="O4">
-        <v>1.000651671762896</v>
+        <v>1.005016521585111</v>
       </c>
       <c r="P4">
-        <v>1.000651671762896</v>
+        <v>1.000413558350021</v>
       </c>
       <c r="Q4">
-        <v>0.9991701661894619</v>
+        <v>1.000413558350021</v>
       </c>
       <c r="R4">
-        <v>0.9991701661894619</v>
+        <v>0.9994955541243569</v>
       </c>
       <c r="S4">
-        <v>0.9967875105731671</v>
+        <v>0.9994955541243569</v>
+      </c>
+      <c r="T4">
+        <v>0.996344821699631</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -687,58 +714,61 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.9918898441950985</v>
+        <v>0.9920719306253711</v>
       </c>
       <c r="D5">
-        <v>1.036780416650421</v>
+        <v>1.036616406673343</v>
       </c>
       <c r="E5">
-        <v>0.9841273185336584</v>
+        <v>0.9841311122394232</v>
       </c>
       <c r="F5">
-        <v>0.9918898441950985</v>
+        <v>0.9920719306253711</v>
       </c>
       <c r="G5">
-        <v>1.022561952621822</v>
+        <v>1.022569247517488</v>
       </c>
       <c r="H5">
-        <v>0.9599438699158646</v>
+        <v>0.9597013650732229</v>
       </c>
       <c r="I5">
-        <v>0.9852842770590969</v>
+        <v>0.9851706286313915</v>
       </c>
       <c r="J5">
-        <v>1.036780416650421</v>
+        <v>1.036616406673343</v>
       </c>
       <c r="K5">
-        <v>0.9918898441950985</v>
+        <v>0.9920719306253711</v>
       </c>
       <c r="L5">
-        <v>1.01045386759204</v>
+        <v>0.9841311122394232</v>
       </c>
       <c r="M5">
-        <v>1.01045386759204</v>
+        <v>1.010373759456383</v>
       </c>
       <c r="N5">
-        <v>1.014489895935301</v>
+        <v>1.010373759456383</v>
       </c>
       <c r="O5">
-        <v>1.004265859793059</v>
+        <v>1.014438922143418</v>
       </c>
       <c r="P5">
-        <v>1.004265859793059</v>
+        <v>1.004273149846046</v>
       </c>
       <c r="Q5">
-        <v>1.001171855893569</v>
+        <v>1.004273149846046</v>
       </c>
       <c r="R5">
-        <v>1.001171855893569</v>
+        <v>1.001222845040877</v>
       </c>
       <c r="S5">
-        <v>0.9967646131626603</v>
+        <v>1.001222845040877</v>
+      </c>
+      <c r="T5">
+        <v>0.9967101151267066</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -746,58 +776,61 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.997720846796156</v>
+        <v>0.9980043998191661</v>
       </c>
       <c r="D6">
-        <v>0.9985576487605068</v>
+        <v>0.9985180596447223</v>
       </c>
       <c r="E6">
-        <v>0.9952626547438717</v>
+        <v>0.9950840607171098</v>
       </c>
       <c r="F6">
-        <v>0.997720846796156</v>
+        <v>0.9980043998191661</v>
       </c>
       <c r="G6">
-        <v>1.000209471210924</v>
+        <v>1.0002790861062</v>
       </c>
       <c r="H6">
-        <v>0.9920254819341123</v>
+        <v>0.9915136988992173</v>
       </c>
       <c r="I6">
-        <v>0.9951913122172871</v>
+        <v>0.995149242567458</v>
       </c>
       <c r="J6">
-        <v>0.9985576487605068</v>
+        <v>0.9985180596447223</v>
       </c>
       <c r="K6">
-        <v>0.997720846796156</v>
+        <v>0.9980043998191661</v>
       </c>
       <c r="L6">
-        <v>0.9969101517521892</v>
+        <v>0.9950840607171098</v>
       </c>
       <c r="M6">
-        <v>0.9969101517521892</v>
+        <v>0.9968010601809161</v>
       </c>
       <c r="N6">
-        <v>0.9980099249051008</v>
+        <v>0.9968010601809161</v>
       </c>
       <c r="O6">
-        <v>0.9971803834335115</v>
+        <v>0.9979604021560107</v>
       </c>
       <c r="P6">
-        <v>0.9971803834335115</v>
+        <v>0.9972021733936661</v>
       </c>
       <c r="Q6">
-        <v>0.9973154992741726</v>
+        <v>0.9972021733936661</v>
       </c>
       <c r="R6">
-        <v>0.9973154992741726</v>
+        <v>0.9974027300000411</v>
       </c>
       <c r="S6">
-        <v>0.996494569277143</v>
+        <v>0.9974027300000411</v>
+      </c>
+      <c r="T6">
+        <v>0.9964247579589789</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -805,55 +838,306 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.9982788055419122</v>
+        <v>1.169935231624025</v>
       </c>
       <c r="D7">
-        <v>0.9956681684574957</v>
+        <v>0.501275923595384</v>
       </c>
       <c r="E7">
-        <v>0.9960100990311169</v>
+        <v>1.088452508488073</v>
       </c>
       <c r="F7">
-        <v>0.9982788055419122</v>
+        <v>1.169935231624025</v>
       </c>
       <c r="G7">
-        <v>0.9986732219721111</v>
+        <v>0.736759667576416</v>
       </c>
       <c r="H7">
-        <v>0.993851654451409</v>
+        <v>1.228842748610638</v>
       </c>
       <c r="I7">
-        <v>0.9959424048917159</v>
+        <v>1.119103383396861</v>
       </c>
       <c r="J7">
-        <v>0.9956681684574957</v>
+        <v>0.501275923595384</v>
       </c>
       <c r="K7">
-        <v>0.9982788055419122</v>
+        <v>1.169935231624025</v>
       </c>
       <c r="L7">
-        <v>0.9958391337443063</v>
+        <v>1.088452508488073</v>
       </c>
       <c r="M7">
-        <v>0.9958391337443063</v>
+        <v>0.7948642160417285</v>
       </c>
       <c r="N7">
-        <v>0.9967838298202413</v>
+        <v>0.7948642160417285</v>
       </c>
       <c r="O7">
-        <v>0.9966523576768416</v>
+        <v>0.7754960332199577</v>
       </c>
       <c r="P7">
-        <v>0.9966523576768417</v>
+        <v>0.9198878879024939</v>
       </c>
       <c r="Q7">
-        <v>0.9970589696431094</v>
+        <v>0.9198878879024939</v>
       </c>
       <c r="R7">
-        <v>0.9970589696431094</v>
+        <v>0.9823997238328765</v>
       </c>
       <c r="S7">
-        <v>0.9964040590576269</v>
+        <v>0.9823997238328765</v>
+      </c>
+      <c r="T7">
+        <v>0.9740615772152328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0.989119581040478</v>
+      </c>
+      <c r="D8">
+        <v>0.9088275117754978</v>
+      </c>
+      <c r="E8">
+        <v>1.030035410330014</v>
+      </c>
+      <c r="F8">
+        <v>0.989119581040478</v>
+      </c>
+      <c r="G8">
+        <v>0.9359611356219023</v>
+      </c>
+      <c r="H8">
+        <v>1.114173862554452</v>
+      </c>
+      <c r="I8">
+        <v>1.024696613891124</v>
+      </c>
+      <c r="J8">
+        <v>0.9088275117754978</v>
+      </c>
+      <c r="K8">
+        <v>0.989119581040478</v>
+      </c>
+      <c r="L8">
+        <v>1.030035410330014</v>
+      </c>
+      <c r="M8">
+        <v>0.9694314610527561</v>
+      </c>
+      <c r="N8">
+        <v>0.9694314610527561</v>
+      </c>
+      <c r="O8">
+        <v>0.9582746859091382</v>
+      </c>
+      <c r="P8">
+        <v>0.9759941677153301</v>
+      </c>
+      <c r="Q8">
+        <v>0.9759941677153301</v>
+      </c>
+      <c r="R8">
+        <v>0.9792755210466171</v>
+      </c>
+      <c r="S8">
+        <v>0.9792755210466171</v>
+      </c>
+      <c r="T8">
+        <v>1.000469019202245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1.97</v>
+      </c>
+      <c r="D9">
+        <v>0.22</v>
+      </c>
+      <c r="E9">
+        <v>0.83</v>
+      </c>
+      <c r="F9">
+        <v>1.97</v>
+      </c>
+      <c r="G9">
+        <v>0.63</v>
+      </c>
+      <c r="H9">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="I9">
+        <v>1.14</v>
+      </c>
+      <c r="J9">
+        <v>0.22</v>
+      </c>
+      <c r="K9">
+        <v>1.97</v>
+      </c>
+      <c r="L9">
+        <v>0.83</v>
+      </c>
+      <c r="M9">
+        <v>0.525</v>
+      </c>
+      <c r="N9">
+        <v>0.525</v>
+      </c>
+      <c r="O9">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="P9">
+        <v>1.006666666666667</v>
+      </c>
+      <c r="Q9">
+        <v>1.006666666666667</v>
+      </c>
+      <c r="R9">
+        <v>1.2475</v>
+      </c>
+      <c r="S9">
+        <v>1.2475</v>
+      </c>
+      <c r="T9">
+        <v>0.9133333333333332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1.33</v>
+      </c>
+      <c r="D10">
+        <v>0.16</v>
+      </c>
+      <c r="E10">
+        <v>1.16</v>
+      </c>
+      <c r="F10">
+        <v>1.33</v>
+      </c>
+      <c r="G10">
+        <v>0.46</v>
+      </c>
+      <c r="H10">
+        <v>1.54</v>
+      </c>
+      <c r="I10">
+        <v>1.22</v>
+      </c>
+      <c r="J10">
+        <v>0.16</v>
+      </c>
+      <c r="K10">
+        <v>1.33</v>
+      </c>
+      <c r="L10">
+        <v>1.16</v>
+      </c>
+      <c r="M10">
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="N10">
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="O10">
+        <v>0.5933333333333333</v>
+      </c>
+      <c r="P10">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="Q10">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="R10">
+        <v>0.995</v>
+      </c>
+      <c r="S10">
+        <v>0.995</v>
+      </c>
+      <c r="T10">
+        <v>0.9783333333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0.9995825844195323</v>
+      </c>
+      <c r="D11">
+        <v>0.9947859823906227</v>
+      </c>
+      <c r="E11">
+        <v>0.9956587129011232</v>
+      </c>
+      <c r="F11">
+        <v>0.9995825844195323</v>
+      </c>
+      <c r="G11">
+        <v>0.9986076548371395</v>
+      </c>
+      <c r="H11">
+        <v>0.9926008551345861</v>
+      </c>
+      <c r="I11">
+        <v>0.9959131770519947</v>
+      </c>
+      <c r="J11">
+        <v>0.9947859823906227</v>
+      </c>
+      <c r="K11">
+        <v>0.9995825844195323</v>
+      </c>
+      <c r="L11">
+        <v>0.9956587129011232</v>
+      </c>
+      <c r="M11">
+        <v>0.9952223476458729</v>
+      </c>
+      <c r="N11">
+        <v>0.9952223476458729</v>
+      </c>
+      <c r="O11">
+        <v>0.9963507833762951</v>
+      </c>
+      <c r="P11">
+        <v>0.9966757599037593</v>
+      </c>
+      <c r="Q11">
+        <v>0.9966757599037593</v>
+      </c>
+      <c r="R11">
+        <v>0.9974024660327026</v>
+      </c>
+      <c r="S11">
+        <v>0.9974024660327026</v>
+      </c>
+      <c r="T11">
+        <v>0.9961914944558329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>